<commit_message>
report, and benchmark results
</commit_message>
<xml_diff>
--- a/analysis/bm_data_plot.xlsx
+++ b/analysis/bm_data_plot.xlsx
@@ -9,14 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="880" yWindow="480" windowWidth="33940" windowHeight="19340" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="33900" windowHeight="19340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>lockfree</t>
   </si>
@@ -52,15 +49,46 @@
   <si>
     <t>spinlock</t>
   </si>
+  <si>
+    <t>Peak Memory Usage</t>
+  </si>
+  <si>
+    <t>Coarse-grained Locking</t>
+  </si>
+  <si>
+    <t>Fine-grained Locking</t>
+  </si>
+  <si>
+    <t>Lock-free</t>
+  </si>
+  <si>
+    <t># Context Switches</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,13 +111,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -640,11 +676,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83709008"/>
-        <c:axId val="83713264"/>
+        <c:axId val="-1880436576"/>
+        <c:axId val="-1880432864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83709008"/>
+        <c:axId val="-1880436576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,12 +792,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83713264"/>
+        <c:crossAx val="-1880432864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83713264"/>
+        <c:axId val="-1880432864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -873,7 +909,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83709008"/>
+        <c:crossAx val="-1880436576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1491,11 +1527,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83752000"/>
-        <c:axId val="83756544"/>
+        <c:axId val="-1881478976"/>
+        <c:axId val="-1881474432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83752000"/>
+        <c:axId val="-1881478976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1532,7 +1568,14 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00111891263354634"/>
+              <c:y val="0.875681257855211"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1598,12 +1641,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83756544"/>
+        <c:crossAx val="-1881474432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83756544"/>
+        <c:axId val="-1881474432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +1758,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83752000"/>
+        <c:crossAx val="-1881478976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2291,11 +2334,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="211544016"/>
-        <c:axId val="211547648"/>
+        <c:axId val="-1881436624"/>
+        <c:axId val="-1881432080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="211544016"/>
+        <c:axId val="-1881436624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2394,7 +2437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211547648"/>
+        <c:crossAx val="-1881432080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2402,7 +2445,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211547648"/>
+        <c:axId val="-1881432080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2508,7 +2551,1388 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211544016"/>
+        <c:crossAx val="-1881436624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Amortized</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Memory Usage</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> per Key-value Pair</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$8:$S$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Coarse-grained Locking</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fine-grained Locking</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lock-free</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$8:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.19224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.644852</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="169"/>
+        <c:axId val="-1652255728"/>
+        <c:axId val="-1652417280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1652255728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1652417280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1652417280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Usage (KB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1652255728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Conext Switches vs. Thread Count</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Coarse-grained Locking</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0209826275028234"/>
+                  <c:y val="0.0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0112983378861357"/>
+                  <c:y val="-2.36607562858263E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0096842896166878"/>
+                  <c:y val="-2.36607562858263E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$9:$AA$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>628.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99954.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101624.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.001613E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.002325E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.000546E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Fine-grained Locking</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00968428961668768"/>
+                  <c:y val="-2.36607562858263E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00484214480834384"/>
+                  <c:y val="0.0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.00645619307779167"/>
+                  <c:y val="-2.36607562858263E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$16:$AA$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1208.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>107974.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>557209.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.002887E6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.005548E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.01524E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Lock-free</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$2:$AA$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1423.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3346.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5237.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6063.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28448.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30477.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="51"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2131055072"/>
+        <c:axId val="-2131052016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2131055072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Thread Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2131052016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2131052016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Conext Switches</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2131055072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2709,6 +4133,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3742,6 +5246,1012 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4279,15 +6789,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>386772</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>48493</xdr:rowOff>
+      <xdr:colOff>376188</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>37909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>404089</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>57728</xdr:rowOff>
+      <xdr:colOff>393505</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>47144</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4308,16 +6818,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>205317</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>675981</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>94186</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>51564</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104769</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4338,91 +6848,69 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>465667</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>10584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>31751</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>455082</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>354246</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>125936</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="H2">
-            <v>1</v>
-          </cell>
-          <cell r="I2">
-            <v>23.4467</v>
-          </cell>
-          <cell r="J2">
-            <v>15.5623</v>
-          </cell>
-          <cell r="K2">
-            <v>18.763000000000002</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="H3">
-            <v>2</v>
-          </cell>
-          <cell r="I3">
-            <v>13.827999999999999</v>
-          </cell>
-          <cell r="J3">
-            <v>21.432200000000002</v>
-          </cell>
-          <cell r="K3">
-            <v>14.3947</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="H4">
-            <v>4</v>
-          </cell>
-          <cell r="I4">
-            <v>9.6289899999999999</v>
-          </cell>
-          <cell r="J4">
-            <v>22.8185</v>
-          </cell>
-          <cell r="K4">
-            <v>15.792</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="H5">
-            <v>8</v>
-          </cell>
-          <cell r="I5">
-            <v>10.6221</v>
-          </cell>
-          <cell r="J5">
-            <v>24.747699999999998</v>
-          </cell>
-          <cell r="K5">
-            <v>21.1647</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6">
-            <v>16</v>
-          </cell>
-          <cell r="I6">
-            <v>14.648199999999999</v>
-          </cell>
-          <cell r="J6">
-            <v>26.049600000000002</v>
-          </cell>
-          <cell r="K6">
-            <v>24.756900000000002</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4688,10 +7176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="H7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="N11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4700,9 +7188,14 @@
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4734,8 +7227,26 @@
         <f>J1/J1</f>
         <v>1</v>
       </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1</v>
       </c>
@@ -4762,8 +7273,20 @@
         <f>J1/J2</f>
         <v>1.7692307692307692</v>
       </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>2649156</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1423</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2</v>
       </c>
@@ -4790,8 +7313,27 @@
         <f>J1/J3</f>
         <v>2.7499999999999996</v>
       </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2635392</v>
+      </c>
+      <c r="S3">
+        <v>2644852</v>
+      </c>
+      <c r="T3">
+        <f>S3/500000</f>
+        <v>5.2897040000000004</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>3346</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>4</v>
       </c>
@@ -4818,8 +7360,27 @@
         <f>J1/J4</f>
         <v>1.8333333333333333</v>
       </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+      <c r="Q4">
+        <v>2644852</v>
+      </c>
+      <c r="S4">
+        <v>96120</v>
+      </c>
+      <c r="T4">
+        <f>S4/500000</f>
+        <v>0.19223999999999999</v>
+      </c>
+      <c r="Z4">
+        <v>4</v>
+      </c>
+      <c r="AA4">
+        <v>5237</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>8</v>
       </c>
@@ -4846,8 +7407,27 @@
         <f>J1/J5</f>
         <v>0.92673992673992667</v>
       </c>
+      <c r="P5">
+        <v>8</v>
+      </c>
+      <c r="Q5">
+        <v>2.38</v>
+      </c>
+      <c r="S5">
+        <v>161280</v>
+      </c>
+      <c r="T5">
+        <f>S5/500000</f>
+        <v>0.32256000000000001</v>
+      </c>
+      <c r="Z5">
+        <v>8</v>
+      </c>
+      <c r="AA5">
+        <v>6063</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>12</v>
       </c>
@@ -4874,8 +7454,20 @@
         <f>J1/J6</f>
         <v>0.61557177615571768</v>
       </c>
+      <c r="P6">
+        <v>12</v>
+      </c>
+      <c r="Q6">
+        <v>3.7</v>
+      </c>
+      <c r="Z6">
+        <v>12</v>
+      </c>
+      <c r="AA6">
+        <v>28448</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>16</v>
       </c>
@@ -4889,8 +7481,28 @@
         <f>C2/C7</f>
         <v>1.6527777777777777</v>
       </c>
+      <c r="P7">
+        <v>16</v>
+      </c>
+      <c r="Q7">
+        <v>2682772</v>
+      </c>
+      <c r="Z7">
+        <v>16</v>
+      </c>
+      <c r="AA7">
+        <v>30477</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8">
+        <v>0.19223999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -4919,8 +7531,32 @@
       <c r="K9">
         <v>2.09</v>
       </c>
+      <c r="O9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="S9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9">
+        <v>0.32256000000000001</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>628</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2</v>
       </c>
@@ -4946,8 +7582,27 @@
       <c r="K10">
         <v>2.78</v>
       </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>5.81</v>
+      </c>
+      <c r="S10" t="s">
+        <v>10</v>
+      </c>
+      <c r="T10">
+        <f>5.289704/2</f>
+        <v>2.6448520000000002</v>
+      </c>
+      <c r="Z10">
+        <v>2</v>
+      </c>
+      <c r="AA10">
+        <v>99954</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>4</v>
       </c>
@@ -4973,8 +7628,20 @@
       <c r="K11">
         <v>4.74</v>
       </c>
+      <c r="P11">
+        <v>4</v>
+      </c>
+      <c r="Q11">
+        <v>6.42</v>
+      </c>
+      <c r="Z11">
+        <v>4</v>
+      </c>
+      <c r="AA11">
+        <v>101624</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>8</v>
       </c>
@@ -5000,8 +7667,20 @@
       <c r="K12">
         <v>4.83</v>
       </c>
+      <c r="P12">
+        <v>8</v>
+      </c>
+      <c r="Q12">
+        <v>6.51</v>
+      </c>
+      <c r="Z12">
+        <v>8</v>
+      </c>
+      <c r="AA12">
+        <v>1001613</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>12</v>
       </c>
@@ -5027,8 +7706,20 @@
       <c r="K13">
         <v>4.8600000000000003</v>
       </c>
+      <c r="P13">
+        <v>12</v>
+      </c>
+      <c r="Q13">
+        <v>6.49</v>
+      </c>
+      <c r="Z13">
+        <v>12</v>
+      </c>
+      <c r="AA13">
+        <v>1002325</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>16</v>
       </c>
@@ -5054,8 +7745,20 @@
       <c r="K14">
         <v>4.83</v>
       </c>
+      <c r="P14">
+        <v>16</v>
+      </c>
+      <c r="Q14">
+        <v>6.64</v>
+      </c>
+      <c r="Z14">
+        <v>16</v>
+      </c>
+      <c r="AA14">
+        <v>1000546</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -5072,8 +7775,26 @@
         <f>C16/C16</f>
         <v>1</v>
       </c>
+      <c r="O16" t="s">
+        <v>4</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>161220</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1208</v>
+      </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>2</v>
       </c>
@@ -5087,8 +7808,20 @@
         <f>C16/C17</f>
         <v>0.75179856115107913</v>
       </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>161280</v>
+      </c>
+      <c r="Z17">
+        <v>2</v>
+      </c>
+      <c r="AA17">
+        <v>107974</v>
+      </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>4</v>
       </c>
@@ -5102,8 +7835,20 @@
         <f>C16/C18</f>
         <v>0.44092827004219404</v>
       </c>
+      <c r="P18">
+        <v>4</v>
+      </c>
+      <c r="Q18">
+        <v>161380</v>
+      </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
+      <c r="AA18">
+        <v>557209</v>
+      </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>8</v>
       </c>
@@ -5117,8 +7862,20 @@
         <f>C16/C19</f>
         <v>0.43271221532091092</v>
       </c>
+      <c r="P19">
+        <v>8</v>
+      </c>
+      <c r="Q19">
+        <v>161348</v>
+      </c>
+      <c r="Z19">
+        <v>8</v>
+      </c>
+      <c r="AA19">
+        <v>1002887</v>
+      </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>12</v>
       </c>
@@ -5132,8 +7889,20 @@
         <f>C16/C20</f>
         <v>0.43004115226337442</v>
       </c>
+      <c r="P20">
+        <v>12</v>
+      </c>
+      <c r="Q20">
+        <v>161612</v>
+      </c>
+      <c r="Z20">
+        <v>12</v>
+      </c>
+      <c r="AA20">
+        <v>1005548</v>
+      </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>16</v>
       </c>
@@ -5146,6 +7915,18 @@
       <c r="F21">
         <f>C16/C21</f>
         <v>0.43271221532091092</v>
+      </c>
+      <c r="P21">
+        <v>16</v>
+      </c>
+      <c r="Q21">
+        <v>161548</v>
+      </c>
+      <c r="Z21">
+        <v>16</v>
+      </c>
+      <c r="AA21">
+        <v>1015240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>